<commit_message>
adapt specs to new validation rules
</commit_message>
<xml_diff>
--- a/spec/fixtures/fichier_usager_test.xlsx
+++ b/spec/fixtures/fichier_usager_test.xlsx
@@ -404,7 +404,7 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -413,7 +413,7 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="60" fontId="6" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -458,7 +458,7 @@
     <xf numFmtId="49" fontId="7" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -473,46 +473,46 @@
     <xf numFmtId="61" fontId="3" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="63" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="63" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="63" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="63" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="63" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="63" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -741,12 +741,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -778,10 +778,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1020,12 +1020,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1329,10 +1329,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1705,7 +1705,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="6">
-        <v>32102</v>
+        <v>29546</v>
       </c>
       <c r="F2" t="s" s="7">
         <v>33</v>

</xml_diff>

<commit_message>
feat(nir): make nir import more secure (#2507)
* make sure nir is coherent with year and civility

* clarified conditions

* fix linter

* adapt specs to new validation rules

* fix unit spec

* fix more specs

* improve condition legibility
</commit_message>
<xml_diff>
--- a/spec/fixtures/fichier_usager_test.xlsx
+++ b/spec/fixtures/fichier_usager_test.xlsx
@@ -404,7 +404,7 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -413,7 +413,7 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="60" fontId="6" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -458,7 +458,7 @@
     <xf numFmtId="49" fontId="7" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -473,46 +473,46 @@
     <xf numFmtId="61" fontId="3" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="63" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="63" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="63" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="63" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="63" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="63" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -741,12 +741,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -778,10 +778,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1020,12 +1020,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1329,10 +1329,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1705,7 +1705,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="6">
-        <v>32102</v>
+        <v>29546</v>
       </c>
       <c r="F2" t="s" s="7">
         <v>33</v>

</xml_diff>